<commit_message>
5th commit-corrected the otp auth
</commit_message>
<xml_diff>
--- a/LifeLink-main/Life/server/data/lifelink_db.xlsx
+++ b/LifeLink-main/Life/server/data/lifelink_db.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -780,20 +780,172 @@
       <c r="K11" t="b">
         <v>1</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11">
         <v>45966.78274959491</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>690ee29e6dfffb265cf88022</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Ashwini Shenoy B</v>
+      </c>
+      <c r="C12" t="str">
+        <v>ashwinishenoyb@gmail.com</v>
+      </c>
+      <c r="D12" t="str">
+        <v>7026438371</v>
+      </c>
+      <c r="E12" t="str">
+        <v>A+</v>
+      </c>
+      <c r="F12" t="str">
+        <v>My Current Location</v>
+      </c>
+      <c r="G12">
+        <v>77.6208384</v>
+      </c>
+      <c r="H12">
+        <v>12.9564672</v>
+      </c>
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>45969.497787939814</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>690ee498bdd4773c2d8f92a9</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Ashwini Shenoy B</v>
+      </c>
+      <c r="C13" t="str">
+        <v>shenoybashwini@gmail.com</v>
+      </c>
+      <c r="D13" t="str">
+        <v>7026438371</v>
+      </c>
+      <c r="E13" t="str">
+        <v>O+</v>
+      </c>
+      <c r="F13" t="str">
+        <v>My Current Location</v>
+      </c>
+      <c r="G13">
+        <v>77.6208384</v>
+      </c>
+      <c r="H13">
+        <v>12.9564672</v>
+      </c>
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" t="b">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>45969.50364131945</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>690ee579bdd4773c2d8f92ae</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Ashwini Shenoy B</v>
+      </c>
+      <c r="C14" t="str">
+        <v>shenoybashwini@gmail.com</v>
+      </c>
+      <c r="D14" t="str">
+        <v>7026438371</v>
+      </c>
+      <c r="E14" t="str">
+        <v>O+</v>
+      </c>
+      <c r="F14" t="str">
+        <v>My Current Location</v>
+      </c>
+      <c r="G14">
+        <v>77.6208384</v>
+      </c>
+      <c r="H14">
+        <v>12.9564672</v>
+      </c>
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" t="b">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>45969.50624263889</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>690ee87057df1e2407c8ae77</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Ashwini Shenoy B</v>
+      </c>
+      <c r="C15" t="str">
+        <v>ashenoyb@gmail.com</v>
+      </c>
+      <c r="D15" t="str">
+        <v>1234567890</v>
+      </c>
+      <c r="E15" t="str">
+        <v>A+</v>
+      </c>
+      <c r="F15" t="str">
+        <v>My Current Location</v>
+      </c>
+      <c r="G15">
+        <v>75.1239547</v>
+      </c>
+      <c r="H15">
+        <v>15.3647083</v>
+      </c>
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" t="b">
+        <v>1</v>
+      </c>
+      <c r="L15" s="1">
+        <v>45969.51502623843</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L15"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1022,9 +1174,41 @@
         <v>45952.68241974537</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>690ee6232f7207491479c1a9</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Ashwini Shenoy B</v>
+      </c>
+      <c r="C8" t="str">
+        <v>ashenoyb@gmail.com</v>
+      </c>
+      <c r="D8" t="str">
+        <v>7026438371</v>
+      </c>
+      <c r="E8" t="str">
+        <v>A+</v>
+      </c>
+      <c r="F8" t="str">
+        <v>mangalore</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8" t="str">
+        <v>Medium</v>
+      </c>
+      <c r="J8">
+        <v>45969.5082124537</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>